<commit_message>
updates to DAC design
</commit_message>
<xml_diff>
--- a/documentation/signals/XEM6310.xlsx
+++ b/documentation/signals/XEM6310.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/eagle/projects/open_covg_daq_pcb/documentation/signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBB628F-EC7B-DB4B-BB92-B93C89D41C3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CCA090-E74B-244E-B491-DB9C16B24F86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32740" yWindow="460" windowWidth="30120" windowHeight="15380" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="30120" windowHeight="18880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XEM6310" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Single DAC Block" sheetId="6" r:id="rId4"/>
     <sheet name="ADC_Range" sheetId="4" r:id="rId5"/>
     <sheet name="Power Supplies" sheetId="7" r:id="rId6"/>
-    <sheet name="todo" sheetId="5" r:id="rId7"/>
+    <sheet name="AC DC wall adapters" sheetId="8" r:id="rId7"/>
+    <sheet name="todo" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="583">
   <si>
     <t>Connector</t>
   </si>
@@ -1778,13 +1779,63 @@
   </si>
   <si>
     <t>"-5V"</t>
+  </si>
+  <si>
+    <r>
+      <t>Product Index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Power Supplies - External/Internal (Off-Board)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>AC DC Desktop, Wall Adapters</t>
+    </r>
+  </si>
+  <si>
+    <t>Some have negative center pin</t>
+  </si>
+  <si>
+    <t>http://catalog.triadmagnetics.com/Asset/WSU120-0700-R.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1926,6 +1977,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2276,7 +2348,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -2286,6 +2358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2644,8 +2717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R147" sqref="R147"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8117,7 +8190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -8242,6 +8315,39 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211B154F-E960-734F-89A4-2CF106292B53}">
+  <dimension ref="A2:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>582</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{18BFC035-E262-2649-8003-46477545F8E9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>

</xml_diff>

<commit_message>
updates to ULP and helper python to create script that labels samtech
</commit_message>
<xml_diff>
--- a/documentation/signals/XEM6310.xlsx
+++ b/documentation/signals/XEM6310.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/eagle/projects/open_covg_daq_pcb/documentation/signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6EEA02-9842-0745-A0B7-9D20698DC15F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61659B67-AA9C-EB47-8D3D-C8C328E580FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="3460" windowWidth="30120" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="560" yWindow="1240" windowWidth="26800" windowHeight="21340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XEM6310" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="585">
   <si>
     <t>Connector</t>
   </si>
@@ -1830,12 +1830,18 @@
   <si>
     <t>http://catalog.triadmagnetics.com/Asset/WSU120-0700-R.pdf</t>
   </si>
+  <si>
+    <t>pVCCO1</t>
+  </si>
+  <si>
+    <t>pVCCO0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1998,6 +2004,13 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2348,7 +2361,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -2359,6 +2372,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2717,14 +2732,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S161"/>
   <sheetViews>
-    <sheetView topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" hidden="1" customWidth="1"/>
     <col min="6" max="9" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" customWidth="1"/>
@@ -3729,9 +3744,8 @@
       <c r="C36" t="s">
         <v>104</v>
       </c>
-      <c r="D36" t="e">
-        <f>+VCCO1</f>
-        <v>#NAME?</v>
+      <c r="D36" s="9" t="s">
+        <v>583</v>
       </c>
       <c r="H36" t="e">
         <f>+VCCO1</f>
@@ -4344,9 +4358,8 @@
       <c r="C56" t="s">
         <v>104</v>
       </c>
-      <c r="D56" t="e">
-        <f>+VCCO1</f>
-        <v>#NAME?</v>
+      <c r="D56" s="9" t="s">
+        <v>583</v>
       </c>
       <c r="H56" t="e">
         <f>+VCCO1</f>
@@ -6058,9 +6071,8 @@
       <c r="C117" t="s">
         <v>316</v>
       </c>
-      <c r="D117" t="e">
-        <f>+VCCO0</f>
-        <v>#NAME?</v>
+      <c r="D117" s="9" t="s">
+        <v>584</v>
       </c>
       <c r="H117" t="e">
         <f>+VCCO0</f>
@@ -6664,9 +6676,8 @@
       <c r="C137" t="s">
         <v>316</v>
       </c>
-      <c r="D137" t="e">
-        <f>+VCCO0</f>
-        <v>#NAME?</v>
+      <c r="D137" s="8" t="s">
+        <v>584</v>
       </c>
       <c r="H137" t="e">
         <f>+VCCO0</f>
@@ -7484,6 +7495,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D36" r:id="rId1" display="+@VCCO1" xr:uid="{1C660438-2532-934B-BF33-A77BADE2CFED}"/>
+    <hyperlink ref="D56" r:id="rId2" display="+@VCCO1" xr:uid="{72F8B25A-F94E-494B-A8DF-CD42567079B6}"/>
+    <hyperlink ref="D117" r:id="rId3" display="+@VCCO1" xr:uid="{F688A4A1-0DC6-6443-B135-39B77771657C}"/>
+    <hyperlink ref="D137" r:id="rId4" display="mailto:+@VCCO1" xr:uid="{EBB14F84-0433-454C-BEF3-69E5544DCCDB}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -7551,7 +7568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates, modified UltraLibrarian footprint for better name placement
</commit_message>
<xml_diff>
--- a/documentation/signals/XEM6310.xlsx
+++ b/documentation/signals/XEM6310.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/eagle/projects/open_covg_daq_pcb/documentation/signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3778D931-8874-404F-AEA0-818F18C82748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51D0F4C-2363-C74B-8170-0B4D0AAA878B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="3460" windowWidth="10600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XEM6310" sheetId="1" r:id="rId1"/>
@@ -7858,7 +7858,7 @@
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8134,7 +8134,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>620</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated pin connection python and the pinout spreadsheet
</commit_message>
<xml_diff>
--- a/documentation/signals/XEM6310.xlsx
+++ b/documentation/signals/XEM6310.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/eagle/projects/open_covg_daq_pcb/documentation/signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51D0F4C-2363-C74B-8170-0B4D0AAA878B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B75D7E8-90FF-0849-8AF3-C55ECC316CD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="3460" windowWidth="10600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39460" yWindow="460" windowWidth="25800" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XEM6310" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="712">
   <si>
     <t>Connector</t>
   </si>
@@ -1946,6 +1946,279 @@
   <si>
     <t>ADP2300</t>
   </si>
+  <si>
+    <t>A0_D-</t>
+  </si>
+  <si>
+    <t>A0_D+</t>
+  </si>
+  <si>
+    <t>A0_DCO-</t>
+  </si>
+  <si>
+    <t>A0_DCO+</t>
+  </si>
+  <si>
+    <t>A0_CLK+</t>
+  </si>
+  <si>
+    <t>A0_EN0</t>
+  </si>
+  <si>
+    <t>lvds</t>
+  </si>
+  <si>
+    <t>lvcmos</t>
+  </si>
+  <si>
+    <t>A0_CNV+</t>
+  </si>
+  <si>
+    <t>A0_CNV-</t>
+  </si>
+  <si>
+    <t>A0_CLK-</t>
+  </si>
+  <si>
+    <t>A1_CNV+</t>
+  </si>
+  <si>
+    <t>A1_CNV-</t>
+  </si>
+  <si>
+    <t>A1_D+</t>
+  </si>
+  <si>
+    <t>A1_D-</t>
+  </si>
+  <si>
+    <t>A1_DCO+</t>
+  </si>
+  <si>
+    <t>A1_EN0</t>
+  </si>
+  <si>
+    <t>A1_DCO-</t>
+  </si>
+  <si>
+    <t>A1_CLK+</t>
+  </si>
+  <si>
+    <t>A1_CLK-</t>
+  </si>
+  <si>
+    <t>A2_CNV+</t>
+  </si>
+  <si>
+    <t>A2_CNV-</t>
+  </si>
+  <si>
+    <t>A2_D+</t>
+  </si>
+  <si>
+    <t>A2_D-</t>
+  </si>
+  <si>
+    <t>A2_DCO+</t>
+  </si>
+  <si>
+    <t>A2_EN0</t>
+  </si>
+  <si>
+    <t>A2_DCO-</t>
+  </si>
+  <si>
+    <t>A2_CLK+</t>
+  </si>
+  <si>
+    <t>A2_CLK-</t>
+  </si>
+  <si>
+    <t>A3_CNV+</t>
+  </si>
+  <si>
+    <t>A3_CNV-</t>
+  </si>
+  <si>
+    <t>A3_D+</t>
+  </si>
+  <si>
+    <t>A3_D-</t>
+  </si>
+  <si>
+    <t>A3_DCO+</t>
+  </si>
+  <si>
+    <t>A3_DCO-</t>
+  </si>
+  <si>
+    <t>A3_CLK+</t>
+  </si>
+  <si>
+    <t>A3_CLK-</t>
+  </si>
+  <si>
+    <t>Schematic sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPGA direction </t>
+  </si>
+  <si>
+    <t>A3_EN0</t>
+  </si>
+  <si>
+    <t>ADCS_SDO</t>
+  </si>
+  <si>
+    <t>ADCS_SDI</t>
+  </si>
+  <si>
+    <t>ADCS_SCLK</t>
+  </si>
+  <si>
+    <t>ADCS_CSB</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>LS_IN0</t>
+  </si>
+  <si>
+    <t>LS_IN1</t>
+  </si>
+  <si>
+    <t>LS_IN2</t>
+  </si>
+  <si>
+    <t>LS_IN3</t>
+  </si>
+  <si>
+    <t>LS_IN4</t>
+  </si>
+  <si>
+    <t>LS_IN5</t>
+  </si>
+  <si>
+    <t>LS0_EN</t>
+  </si>
+  <si>
+    <t>LS1_EN</t>
+  </si>
+  <si>
+    <t>A_EN2_HV</t>
+  </si>
+  <si>
+    <t>D3_SDI</t>
+  </si>
+  <si>
+    <t>D3_CSB</t>
+  </si>
+  <si>
+    <t>D3_SCLK</t>
+  </si>
+  <si>
+    <t>D2_CSB</t>
+  </si>
+  <si>
+    <t>D2_SDI</t>
+  </si>
+  <si>
+    <t>D2_SCLK</t>
+  </si>
+  <si>
+    <t>D0_CSB</t>
+  </si>
+  <si>
+    <t>D0_SDI</t>
+  </si>
+  <si>
+    <t>D0_SCLK</t>
+  </si>
+  <si>
+    <t>D1_CSB</t>
+  </si>
+  <si>
+    <t>D1_SDI</t>
+  </si>
+  <si>
+    <t>D1_SCLK</t>
+  </si>
+  <si>
+    <t>DS_SDA</t>
+  </si>
+  <si>
+    <t>DS_SCL</t>
+  </si>
+  <si>
+    <t>DS_CLRB</t>
+  </si>
+  <si>
+    <t>INOUT</t>
+  </si>
+  <si>
+    <t>A_EN1</t>
+  </si>
+  <si>
+    <t>A_EN3</t>
+  </si>
+  <si>
+    <t>GPIO_3V3_0</t>
+  </si>
+  <si>
+    <t>GPIO_3V3_1</t>
+  </si>
+  <si>
+    <t>GPIO_3V3_2</t>
+  </si>
+  <si>
+    <t>GP_0</t>
+  </si>
+  <si>
+    <t>GP_1</t>
+  </si>
+  <si>
+    <t>GP_2</t>
+  </si>
+  <si>
+    <t>GP_3</t>
+  </si>
+  <si>
+    <t>GP_4</t>
+  </si>
+  <si>
+    <t>GP_5</t>
+  </si>
+  <si>
+    <t>GP_6</t>
+  </si>
+  <si>
+    <t>GP_7</t>
+  </si>
+  <si>
+    <t>GP_8</t>
+  </si>
+  <si>
+    <t>GP_9</t>
+  </si>
+  <si>
+    <t>GP_10</t>
+  </si>
+  <si>
+    <t>GP_11</t>
+  </si>
+  <si>
+    <t>GP_SDA</t>
+  </si>
+  <si>
+    <t>GP_SCL</t>
+  </si>
+  <si>
+    <t>NET</t>
+  </si>
 </sst>
 </file>
 
@@ -1954,7 +2227,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2121,6 +2394,13 @@
     <font>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2474,7 +2754,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -2489,6 +2769,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="42" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2845,26 +3126,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S161"/>
+  <dimension ref="A1:W161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" hidden="1" customWidth="1"/>
-    <col min="6" max="9" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="10" width="10.83203125" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="14.5" hidden="1" customWidth="1"/>
     <col min="13" max="17" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="18" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2919,8 +3202,17 @@
       <c r="R1" s="1" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T1" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2940,7 +3232,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2960,7 +3252,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2980,7 +3272,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -3000,7 +3292,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3020,7 +3312,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3040,7 +3332,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -3060,7 +3352,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3080,7 +3372,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3100,7 +3392,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3123,7 +3415,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3151,8 +3443,20 @@
       <c r="S12" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T12" t="s">
+        <v>693</v>
+      </c>
+      <c r="U12">
+        <v>3</v>
+      </c>
+      <c r="V12" t="s">
+        <v>666</v>
+      </c>
+      <c r="W12" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3175,7 +3479,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3198,7 +3502,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -3221,7 +3525,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -3253,7 +3557,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -3284,8 +3588,20 @@
       <c r="R17" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T17" t="s">
+        <v>661</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17" t="s">
+        <v>665</v>
+      </c>
+      <c r="W17" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -3316,8 +3632,20 @@
       <c r="R18" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T18" t="s">
+        <v>667</v>
+      </c>
+      <c r="U18">
+        <v>3</v>
+      </c>
+      <c r="V18" t="s">
+        <v>666</v>
+      </c>
+      <c r="W18" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3348,8 +3676,20 @@
       <c r="R19" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T19" t="s">
+        <v>662</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19" t="s">
+        <v>666</v>
+      </c>
+      <c r="W19" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3377,8 +3717,20 @@
       <c r="R20" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T20" t="s">
+        <v>668</v>
+      </c>
+      <c r="U20">
+        <v>3</v>
+      </c>
+      <c r="V20" t="s">
+        <v>666</v>
+      </c>
+      <c r="W20" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -3406,8 +3758,20 @@
       <c r="R21" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T21" t="s">
+        <v>663</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21" t="s">
+        <v>666</v>
+      </c>
+      <c r="W21" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -3438,8 +3802,20 @@
       <c r="R22" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T22" t="s">
+        <v>669</v>
+      </c>
+      <c r="U22">
+        <v>3</v>
+      </c>
+      <c r="V22" t="s">
+        <v>666</v>
+      </c>
+      <c r="W22" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -3470,8 +3846,20 @@
       <c r="R23" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T23" t="s">
+        <v>664</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23" t="s">
+        <v>666</v>
+      </c>
+      <c r="W23" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -3502,8 +3890,20 @@
       <c r="R24" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T24" t="s">
+        <v>670</v>
+      </c>
+      <c r="U24">
+        <v>3</v>
+      </c>
+      <c r="V24" t="s">
+        <v>666</v>
+      </c>
+      <c r="W24" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -3534,8 +3934,20 @@
       <c r="R25" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T25" t="s">
+        <v>671</v>
+      </c>
+      <c r="U25">
+        <v>3</v>
+      </c>
+      <c r="V25" t="s">
+        <v>666</v>
+      </c>
+      <c r="W25" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -3566,8 +3978,20 @@
       <c r="R26" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T26" t="s">
+        <v>672</v>
+      </c>
+      <c r="U26">
+        <v>3</v>
+      </c>
+      <c r="V26" t="s">
+        <v>666</v>
+      </c>
+      <c r="W26" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -3599,7 +4023,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -3630,8 +4054,20 @@
       <c r="R28" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T28" t="s">
+        <v>677</v>
+      </c>
+      <c r="U28">
+        <v>11</v>
+      </c>
+      <c r="V28" t="s">
+        <v>666</v>
+      </c>
+      <c r="W28" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -3662,8 +4098,20 @@
       <c r="R29" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T29" t="s">
+        <v>688</v>
+      </c>
+      <c r="U29">
+        <v>12</v>
+      </c>
+      <c r="V29" t="s">
+        <v>691</v>
+      </c>
+      <c r="W29" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -3694,8 +4142,20 @@
       <c r="R30" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T30" t="s">
+        <v>676</v>
+      </c>
+      <c r="U30">
+        <v>11</v>
+      </c>
+      <c r="V30" t="s">
+        <v>666</v>
+      </c>
+      <c r="W30" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -3726,8 +4186,20 @@
       <c r="R31" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T31" t="s">
+        <v>689</v>
+      </c>
+      <c r="U31">
+        <v>12</v>
+      </c>
+      <c r="V31" t="s">
+        <v>691</v>
+      </c>
+      <c r="W31" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -3755,8 +4227,20 @@
       <c r="R32" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T32" t="s">
+        <v>678</v>
+      </c>
+      <c r="U32">
+        <v>11</v>
+      </c>
+      <c r="V32" t="s">
+        <v>666</v>
+      </c>
+      <c r="W32" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -3784,8 +4268,20 @@
       <c r="R33" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T33" t="s">
+        <v>690</v>
+      </c>
+      <c r="U33">
+        <v>12</v>
+      </c>
+      <c r="V33" t="s">
+        <v>691</v>
+      </c>
+      <c r="W33" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -3816,8 +4312,20 @@
       <c r="R34" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T34" t="s">
+        <v>679</v>
+      </c>
+      <c r="U34">
+        <v>10</v>
+      </c>
+      <c r="V34" t="s">
+        <v>666</v>
+      </c>
+      <c r="W34" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -3849,7 +4357,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -3876,7 +4384,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -3899,7 +4407,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -3930,8 +4438,20 @@
       <c r="R38" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T38" t="s">
+        <v>680</v>
+      </c>
+      <c r="U38">
+        <v>10</v>
+      </c>
+      <c r="V38" t="s">
+        <v>666</v>
+      </c>
+      <c r="W38" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -3966,7 +4486,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -3997,8 +4517,20 @@
       <c r="R40" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T40" t="s">
+        <v>681</v>
+      </c>
+      <c r="U40">
+        <v>10</v>
+      </c>
+      <c r="V40" t="s">
+        <v>666</v>
+      </c>
+      <c r="W40" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -4033,7 +4565,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -4061,8 +4593,20 @@
       <c r="R42" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T42" t="s">
+        <v>682</v>
+      </c>
+      <c r="U42">
+        <v>8</v>
+      </c>
+      <c r="V42" t="s">
+        <v>666</v>
+      </c>
+      <c r="W42" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -4091,7 +4635,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -4122,8 +4666,20 @@
       <c r="R44" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T44" t="s">
+        <v>683</v>
+      </c>
+      <c r="U44">
+        <v>8</v>
+      </c>
+      <c r="V44" t="s">
+        <v>666</v>
+      </c>
+      <c r="W44" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -4155,7 +4711,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -4186,8 +4742,20 @@
       <c r="R46" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T46" t="s">
+        <v>684</v>
+      </c>
+      <c r="U46">
+        <v>8</v>
+      </c>
+      <c r="V46" t="s">
+        <v>666</v>
+      </c>
+      <c r="W46" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -4219,7 +4787,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -4250,8 +4818,20 @@
       <c r="R48" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T48" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="U48" s="12">
+        <v>11</v>
+      </c>
+      <c r="V48" s="12" t="s">
+        <v>666</v>
+      </c>
+      <c r="W48" s="12" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -4282,8 +4862,12 @@
       <c r="R49" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T49" s="12"/>
+      <c r="U49" s="12"/>
+      <c r="V49" s="12"/>
+      <c r="W49" s="12"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -4311,8 +4895,20 @@
       <c r="R50" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T50" s="12" t="s">
+        <v>686</v>
+      </c>
+      <c r="U50" s="12">
+        <v>11</v>
+      </c>
+      <c r="V50" s="12" t="s">
+        <v>666</v>
+      </c>
+      <c r="W50" s="12" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -4340,8 +4936,12 @@
       <c r="R51" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T51" s="12"/>
+      <c r="U51" s="12"/>
+      <c r="V51" s="12"/>
+      <c r="W51" s="12"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -4369,8 +4969,20 @@
       <c r="R52" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T52" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="U52" s="12">
+        <v>11</v>
+      </c>
+      <c r="V52" s="12" t="s">
+        <v>666</v>
+      </c>
+      <c r="W52" s="12" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -4399,7 +5011,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -4428,7 +5040,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -4463,7 +5075,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -4490,7 +5102,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -4510,7 +5122,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -4538,8 +5150,20 @@
       <c r="R58" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T58" t="s">
+        <v>694</v>
+      </c>
+      <c r="U58">
+        <v>3</v>
+      </c>
+      <c r="V58" t="s">
+        <v>666</v>
+      </c>
+      <c r="W58" s="12" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -4573,8 +5197,20 @@
       <c r="R59" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T59" t="s">
+        <v>695</v>
+      </c>
+      <c r="U59">
+        <v>3</v>
+      </c>
+      <c r="V59" t="s">
+        <v>666</v>
+      </c>
+      <c r="W59" s="12" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -4608,8 +5244,20 @@
       <c r="R60" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T60" t="s">
+        <v>696</v>
+      </c>
+      <c r="U60">
+        <v>3</v>
+      </c>
+      <c r="V60" t="s">
+        <v>666</v>
+      </c>
+      <c r="W60" s="12" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -4637,8 +5285,20 @@
       <c r="R61" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T61" t="s">
+        <v>697</v>
+      </c>
+      <c r="U61">
+        <v>2</v>
+      </c>
+      <c r="V61" t="s">
+        <v>666</v>
+      </c>
+      <c r="W61" s="12" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -4672,8 +5332,17 @@
       <c r="R62" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T62" t="s">
+        <v>698</v>
+      </c>
+      <c r="U62">
+        <v>2</v>
+      </c>
+      <c r="V62" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -4704,8 +5373,17 @@
       <c r="R63" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T63" t="s">
+        <v>699</v>
+      </c>
+      <c r="U63">
+        <v>2</v>
+      </c>
+      <c r="V63" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -4736,8 +5414,17 @@
       <c r="R64" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T64" t="s">
+        <v>700</v>
+      </c>
+      <c r="U64">
+        <v>2</v>
+      </c>
+      <c r="V64" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -4768,8 +5455,17 @@
       <c r="R65" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T65" t="s">
+        <v>701</v>
+      </c>
+      <c r="U65">
+        <v>2</v>
+      </c>
+      <c r="V65" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -4800,8 +5496,17 @@
       <c r="R66" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T66" t="s">
+        <v>702</v>
+      </c>
+      <c r="U66">
+        <v>2</v>
+      </c>
+      <c r="V66" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -4832,8 +5537,17 @@
       <c r="R67" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T67" t="s">
+        <v>703</v>
+      </c>
+      <c r="U67">
+        <v>2</v>
+      </c>
+      <c r="V67" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>17</v>
       </c>
@@ -4864,8 +5578,17 @@
       <c r="R68" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T68" t="s">
+        <v>704</v>
+      </c>
+      <c r="U68">
+        <v>2</v>
+      </c>
+      <c r="V68" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>17</v>
       </c>
@@ -4896,8 +5619,17 @@
       <c r="R69" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T69" t="s">
+        <v>705</v>
+      </c>
+      <c r="U69">
+        <v>2</v>
+      </c>
+      <c r="V69" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>17</v>
       </c>
@@ -4928,8 +5660,17 @@
       <c r="R70" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T70" t="s">
+        <v>706</v>
+      </c>
+      <c r="U70">
+        <v>2</v>
+      </c>
+      <c r="V70" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>17</v>
       </c>
@@ -4960,8 +5701,17 @@
       <c r="R71" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T71" t="s">
+        <v>707</v>
+      </c>
+      <c r="U71">
+        <v>2</v>
+      </c>
+      <c r="V71" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>17</v>
       </c>
@@ -4992,8 +5742,17 @@
       <c r="R72" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T72" t="s">
+        <v>708</v>
+      </c>
+      <c r="U72">
+        <v>2</v>
+      </c>
+      <c r="V72" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>17</v>
       </c>
@@ -5024,8 +5783,17 @@
       <c r="R73" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T73" t="s">
+        <v>709</v>
+      </c>
+      <c r="U73">
+        <v>2</v>
+      </c>
+      <c r="V73" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>17</v>
       </c>
@@ -5056,8 +5824,17 @@
       <c r="R74" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T74" t="s">
+        <v>710</v>
+      </c>
+      <c r="U74">
+        <v>2</v>
+      </c>
+      <c r="V74" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>17</v>
       </c>
@@ -5089,7 +5866,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>17</v>
       </c>
@@ -5121,7 +5898,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>17</v>
       </c>
@@ -5153,7 +5930,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -5188,7 +5965,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -5208,7 +5985,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -5243,7 +6020,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -5263,7 +6040,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>232</v>
       </c>
@@ -5287,7 +6064,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>232</v>
       </c>
@@ -5304,7 +6081,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>232</v>
       </c>
@@ -5325,7 +6102,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>232</v>
       </c>
@@ -5342,7 +6119,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>232</v>
       </c>
@@ -5363,7 +6140,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>232</v>
       </c>
@@ -5380,7 +6157,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>232</v>
       </c>
@@ -5400,7 +6177,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>232</v>
       </c>
@@ -5422,8 +6199,20 @@
       <c r="M89" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T89" t="s">
+        <v>673</v>
+      </c>
+      <c r="U89">
+        <v>3</v>
+      </c>
+      <c r="V89" t="s">
+        <v>666</v>
+      </c>
+      <c r="W89" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>232</v>
       </c>
@@ -5443,7 +6232,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>232</v>
       </c>
@@ -5465,8 +6254,20 @@
       <c r="M91" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T91" t="s">
+        <v>674</v>
+      </c>
+      <c r="U91">
+        <v>3</v>
+      </c>
+      <c r="V91" t="s">
+        <v>666</v>
+      </c>
+      <c r="W91" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>232</v>
       </c>
@@ -5486,7 +6287,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>232</v>
       </c>
@@ -5508,8 +6309,20 @@
       <c r="M93" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T93" t="s">
+        <v>692</v>
+      </c>
+      <c r="U93">
+        <v>3</v>
+      </c>
+      <c r="V93" t="s">
+        <v>666</v>
+      </c>
+      <c r="W93" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>232</v>
       </c>
@@ -5529,7 +6342,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>232</v>
       </c>
@@ -5546,7 +6359,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>232</v>
       </c>
@@ -5578,7 +6391,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>232</v>
       </c>
@@ -5607,7 +6420,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>232</v>
       </c>
@@ -5639,7 +6452,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>232</v>
       </c>
@@ -5668,7 +6481,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>232</v>
       </c>
@@ -5700,7 +6513,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>232</v>
       </c>
@@ -5729,7 +6542,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>232</v>
       </c>
@@ -5761,7 +6574,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>232</v>
       </c>
@@ -5790,7 +6603,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>232</v>
       </c>
@@ -5821,8 +6634,20 @@
       <c r="R104" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T104" t="s">
+        <v>629</v>
+      </c>
+      <c r="U104">
+        <v>4</v>
+      </c>
+      <c r="V104" t="s">
+        <v>486</v>
+      </c>
+      <c r="W104" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>232</v>
       </c>
@@ -5851,7 +6676,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>232</v>
       </c>
@@ -5882,8 +6707,20 @@
       <c r="R106" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T106" t="s">
+        <v>630</v>
+      </c>
+      <c r="U106">
+        <v>4</v>
+      </c>
+      <c r="V106" t="s">
+        <v>486</v>
+      </c>
+      <c r="W106" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>232</v>
       </c>
@@ -5912,7 +6749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>232</v>
       </c>
@@ -5943,8 +6780,20 @@
       <c r="R108" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T108" t="s">
+        <v>622</v>
+      </c>
+      <c r="U108">
+        <v>4</v>
+      </c>
+      <c r="V108" t="s">
+        <v>484</v>
+      </c>
+      <c r="W108" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>232</v>
       </c>
@@ -5973,7 +6822,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>232</v>
       </c>
@@ -6004,8 +6853,20 @@
       <c r="R110" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T110" t="s">
+        <v>621</v>
+      </c>
+      <c r="U110">
+        <v>4</v>
+      </c>
+      <c r="V110" t="s">
+        <v>484</v>
+      </c>
+      <c r="W110" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>232</v>
       </c>
@@ -6034,7 +6895,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>232</v>
       </c>
@@ -6065,8 +6926,20 @@
       <c r="R112" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T112" t="s">
+        <v>624</v>
+      </c>
+      <c r="U112">
+        <v>4</v>
+      </c>
+      <c r="V112" t="s">
+        <v>484</v>
+      </c>
+      <c r="W112" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>232</v>
       </c>
@@ -6094,8 +6967,20 @@
       <c r="P113" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T113" t="s">
+        <v>626</v>
+      </c>
+      <c r="U113">
+        <v>4</v>
+      </c>
+      <c r="V113" t="s">
+        <v>486</v>
+      </c>
+      <c r="W113" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>232</v>
       </c>
@@ -6126,8 +7011,20 @@
       <c r="R114" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T114" t="s">
+        <v>623</v>
+      </c>
+      <c r="U114">
+        <v>4</v>
+      </c>
+      <c r="V114" t="s">
+        <v>484</v>
+      </c>
+      <c r="W114" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>232</v>
       </c>
@@ -6155,8 +7052,20 @@
       <c r="P115" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T115" t="s">
+        <v>675</v>
+      </c>
+      <c r="U115">
+        <v>3</v>
+      </c>
+      <c r="V115" t="s">
+        <v>666</v>
+      </c>
+      <c r="W115" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>232</v>
       </c>
@@ -6176,7 +7085,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>232</v>
       </c>
@@ -6200,7 +7109,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>232</v>
       </c>
@@ -6231,8 +7140,20 @@
       <c r="R118" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T118" t="s">
+        <v>625</v>
+      </c>
+      <c r="U118">
+        <v>4</v>
+      </c>
+      <c r="V118" t="s">
+        <v>484</v>
+      </c>
+      <c r="W118" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>232</v>
       </c>
@@ -6261,7 +7182,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>232</v>
       </c>
@@ -6292,8 +7213,20 @@
       <c r="R120" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T120" t="s">
+        <v>631</v>
+      </c>
+      <c r="U120">
+        <v>4</v>
+      </c>
+      <c r="V120" t="s">
+        <v>484</v>
+      </c>
+      <c r="W120" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="121" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>232</v>
       </c>
@@ -6322,7 +7255,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>232</v>
       </c>
@@ -6354,7 +7287,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>232</v>
       </c>
@@ -6386,7 +7319,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>232</v>
       </c>
@@ -6418,7 +7351,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>232</v>
       </c>
@@ -6450,7 +7383,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>232</v>
       </c>
@@ -6482,7 +7415,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>232</v>
       </c>
@@ -6510,8 +7443,20 @@
       <c r="P127" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T127" t="s">
+        <v>632</v>
+      </c>
+      <c r="U127">
+        <v>5</v>
+      </c>
+      <c r="V127" t="s">
+        <v>486</v>
+      </c>
+      <c r="W127" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>232</v>
       </c>
@@ -6543,7 +7488,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>232</v>
       </c>
@@ -6571,8 +7516,20 @@
       <c r="P129" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T129" t="s">
+        <v>633</v>
+      </c>
+      <c r="U129">
+        <v>5</v>
+      </c>
+      <c r="V129" t="s">
+        <v>486</v>
+      </c>
+      <c r="W129" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="130" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>232</v>
       </c>
@@ -6604,7 +7561,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>232</v>
       </c>
@@ -6632,8 +7589,20 @@
       <c r="P131" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T131" t="s">
+        <v>634</v>
+      </c>
+      <c r="U131">
+        <v>5</v>
+      </c>
+      <c r="V131" t="s">
+        <v>484</v>
+      </c>
+      <c r="W131" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="132" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>232</v>
       </c>
@@ -6665,7 +7634,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>232</v>
       </c>
@@ -6696,8 +7665,20 @@
       <c r="P133" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T133" t="s">
+        <v>635</v>
+      </c>
+      <c r="U133">
+        <v>5</v>
+      </c>
+      <c r="V133" t="s">
+        <v>484</v>
+      </c>
+      <c r="W133" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="134" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>232</v>
       </c>
@@ -6729,7 +7710,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>232</v>
       </c>
@@ -6760,8 +7741,20 @@
       <c r="P135" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T135" t="s">
+        <v>636</v>
+      </c>
+      <c r="U135">
+        <v>5</v>
+      </c>
+      <c r="V135" t="s">
+        <v>484</v>
+      </c>
+      <c r="W135" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="136" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>232</v>
       </c>
@@ -6781,7 +7774,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>232</v>
       </c>
@@ -6805,7 +7798,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>232</v>
       </c>
@@ -6836,8 +7829,20 @@
       <c r="R138" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T138" t="s">
+        <v>637</v>
+      </c>
+      <c r="U138">
+        <v>5</v>
+      </c>
+      <c r="V138" t="s">
+        <v>486</v>
+      </c>
+      <c r="W138" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="139" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>232</v>
       </c>
@@ -6868,8 +7873,20 @@
       <c r="P139" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T139" t="s">
+        <v>638</v>
+      </c>
+      <c r="U139">
+        <v>5</v>
+      </c>
+      <c r="V139" t="s">
+        <v>484</v>
+      </c>
+      <c r="W139" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="140" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>232</v>
       </c>
@@ -6903,8 +7920,20 @@
       <c r="R140" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T140" t="s">
+        <v>639</v>
+      </c>
+      <c r="U140">
+        <v>5</v>
+      </c>
+      <c r="V140" t="s">
+        <v>484</v>
+      </c>
+      <c r="W140" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="141" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>232</v>
       </c>
@@ -6935,8 +7964,20 @@
       <c r="P141" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T141" t="s">
+        <v>650</v>
+      </c>
+      <c r="U141">
+        <v>7</v>
+      </c>
+      <c r="V141" t="s">
+        <v>486</v>
+      </c>
+      <c r="W141" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="142" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>232</v>
       </c>
@@ -6970,8 +8011,20 @@
       <c r="R142" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T142" t="s">
+        <v>640</v>
+      </c>
+      <c r="U142">
+        <v>5</v>
+      </c>
+      <c r="V142" t="s">
+        <v>484</v>
+      </c>
+      <c r="W142" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="143" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>232</v>
       </c>
@@ -7002,8 +8055,20 @@
       <c r="P143" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T143" t="s">
+        <v>651</v>
+      </c>
+      <c r="U143">
+        <v>7</v>
+      </c>
+      <c r="V143" t="s">
+        <v>486</v>
+      </c>
+      <c r="W143" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="144" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>232</v>
       </c>
@@ -7037,8 +8102,20 @@
       <c r="R144" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T144" t="s">
+        <v>641</v>
+      </c>
+      <c r="U144">
+        <v>6</v>
+      </c>
+      <c r="V144" t="s">
+        <v>486</v>
+      </c>
+      <c r="W144" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="145" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>232</v>
       </c>
@@ -7072,8 +8149,20 @@
       <c r="P145" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T145" t="s">
+        <v>652</v>
+      </c>
+      <c r="U145">
+        <v>7</v>
+      </c>
+      <c r="V145" t="s">
+        <v>484</v>
+      </c>
+      <c r="W145" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="146" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>232</v>
       </c>
@@ -7107,8 +8196,20 @@
       <c r="R146" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T146" t="s">
+        <v>642</v>
+      </c>
+      <c r="U146">
+        <v>6</v>
+      </c>
+      <c r="V146" t="s">
+        <v>486</v>
+      </c>
+      <c r="W146" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="147" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>232</v>
       </c>
@@ -7142,8 +8243,20 @@
       <c r="P147" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T147" t="s">
+        <v>653</v>
+      </c>
+      <c r="U147">
+        <v>7</v>
+      </c>
+      <c r="V147" t="s">
+        <v>484</v>
+      </c>
+      <c r="W147" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="148" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>232</v>
       </c>
@@ -7177,8 +8290,20 @@
       <c r="R148" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T148" t="s">
+        <v>643</v>
+      </c>
+      <c r="U148">
+        <v>6</v>
+      </c>
+      <c r="V148" t="s">
+        <v>484</v>
+      </c>
+      <c r="W148" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="149" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>232</v>
       </c>
@@ -7212,8 +8337,20 @@
       <c r="R149" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T149" t="s">
+        <v>654</v>
+      </c>
+      <c r="U149">
+        <v>7</v>
+      </c>
+      <c r="V149" t="s">
+        <v>484</v>
+      </c>
+      <c r="W149" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="150" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>232</v>
       </c>
@@ -7247,8 +8384,20 @@
       <c r="R150" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T150" t="s">
+        <v>644</v>
+      </c>
+      <c r="U150">
+        <v>6</v>
+      </c>
+      <c r="V150" t="s">
+        <v>484</v>
+      </c>
+      <c r="W150" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="151" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>232</v>
       </c>
@@ -7282,8 +8431,20 @@
       <c r="R151" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T151" t="s">
+        <v>655</v>
+      </c>
+      <c r="U151" s="12">
+        <v>7</v>
+      </c>
+      <c r="V151" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="W151" s="12" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="152" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>232</v>
       </c>
@@ -7317,8 +8478,20 @@
       <c r="R152" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T152" t="s">
+        <v>645</v>
+      </c>
+      <c r="U152">
+        <v>6</v>
+      </c>
+      <c r="V152" t="s">
+        <v>484</v>
+      </c>
+      <c r="W152" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="153" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>232</v>
       </c>
@@ -7352,8 +8525,20 @@
       <c r="R153" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T153" t="s">
+        <v>646</v>
+      </c>
+      <c r="U153">
+        <v>6</v>
+      </c>
+      <c r="V153" t="s">
+        <v>486</v>
+      </c>
+      <c r="W153" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="154" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>232</v>
       </c>
@@ -7387,8 +8572,20 @@
       <c r="R154" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T154" t="s">
+        <v>647</v>
+      </c>
+      <c r="U154">
+        <v>6</v>
+      </c>
+      <c r="V154" t="s">
+        <v>484</v>
+      </c>
+      <c r="W154" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="155" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>232</v>
       </c>
@@ -7422,8 +8619,20 @@
       <c r="R155" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T155" t="s">
+        <v>660</v>
+      </c>
+      <c r="U155">
+        <v>7</v>
+      </c>
+      <c r="V155" t="s">
+        <v>486</v>
+      </c>
+      <c r="W155" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="156" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>232</v>
       </c>
@@ -7457,8 +8666,20 @@
       <c r="R156" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T156" t="s">
+        <v>649</v>
+      </c>
+      <c r="U156">
+        <v>6</v>
+      </c>
+      <c r="V156" t="s">
+        <v>484</v>
+      </c>
+      <c r="W156" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="157" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>232</v>
       </c>
@@ -7492,8 +8713,20 @@
       <c r="R157" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T157" t="s">
+        <v>648</v>
+      </c>
+      <c r="U157">
+        <v>6</v>
+      </c>
+      <c r="V157" t="s">
+        <v>484</v>
+      </c>
+      <c r="W157" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="158" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>232</v>
       </c>
@@ -7530,8 +8763,20 @@
       <c r="R158" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T158" t="s">
+        <v>656</v>
+      </c>
+      <c r="U158">
+        <v>7</v>
+      </c>
+      <c r="V158" t="s">
+        <v>484</v>
+      </c>
+      <c r="W158" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="159" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>232</v>
       </c>
@@ -7551,7 +8796,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>232</v>
       </c>
@@ -7587,6 +8832,18 @@
       </c>
       <c r="R160" t="s">
         <v>562</v>
+      </c>
+      <c r="T160" t="s">
+        <v>657</v>
+      </c>
+      <c r="U160">
+        <v>7</v>
+      </c>
+      <c r="V160" t="s">
+        <v>484</v>
+      </c>
+      <c r="W160" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.2">
@@ -7857,7 +9114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
cleared PCB DRC errors
</commit_message>
<xml_diff>
--- a/documentation/signals/XEM6310.xlsx
+++ b/documentation/signals/XEM6310.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/eagle/projects/open_covg_daq_pcb/documentation/signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B75D7E8-90FF-0849-8AF3-C55ECC316CD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E613CAD9-E7A9-DA46-AF77-EAB73A006553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39460" yWindow="460" windowWidth="25800" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XEM6310" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="713">
   <si>
     <t>Connector</t>
   </si>
@@ -1962,9 +1962,6 @@
     <t>A0_CLK+</t>
   </si>
   <si>
-    <t>A0_EN0</t>
-  </si>
-  <si>
     <t>lvds</t>
   </si>
   <si>
@@ -1995,9 +1992,6 @@
     <t>A1_DCO+</t>
   </si>
   <si>
-    <t>A1_EN0</t>
-  </si>
-  <si>
     <t>A1_DCO-</t>
   </si>
   <si>
@@ -2022,9 +2016,6 @@
     <t>A2_DCO+</t>
   </si>
   <si>
-    <t>A2_EN0</t>
-  </si>
-  <si>
     <t>A2_DCO-</t>
   </si>
   <si>
@@ -2106,9 +2097,6 @@
     <t>LS0_EN</t>
   </si>
   <si>
-    <t>LS1_EN</t>
-  </si>
-  <si>
     <t>A_EN2_HV</t>
   </si>
   <si>
@@ -2218,6 +2206,21 @@
   </si>
   <si>
     <t>NET</t>
+  </si>
+  <si>
+    <t>A0_EN0_HV</t>
+  </si>
+  <si>
+    <t>A1_EN0_HV</t>
+  </si>
+  <si>
+    <t>A2_EN0_HV</t>
+  </si>
+  <si>
+    <t>A3_EN0_HV</t>
+  </si>
+  <si>
+    <t>JP1-10</t>
   </si>
 </sst>
 </file>
@@ -3128,8 +3131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="T92" sqref="T92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3203,13 +3206,13 @@
         <v>561</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -3444,13 +3447,13 @@
         <v>564</v>
       </c>
       <c r="T12" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="U12">
         <v>3</v>
       </c>
       <c r="V12" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W12" t="s">
         <v>518</v>
@@ -3589,13 +3592,13 @@
         <v>562</v>
       </c>
       <c r="T17" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="U17">
         <v>1</v>
       </c>
       <c r="V17" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="W17" t="s">
         <v>518</v>
@@ -3633,13 +3636,13 @@
         <v>562</v>
       </c>
       <c r="T18" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="U18">
         <v>3</v>
       </c>
       <c r="V18" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W18" t="s">
         <v>518</v>
@@ -3677,13 +3680,13 @@
         <v>562</v>
       </c>
       <c r="T19" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="U19">
         <v>1</v>
       </c>
       <c r="V19" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W19" t="s">
         <v>518</v>
@@ -3718,13 +3721,13 @@
         <v>562</v>
       </c>
       <c r="T20" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="U20">
         <v>3</v>
       </c>
       <c r="V20" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W20" t="s">
         <v>518</v>
@@ -3759,13 +3762,13 @@
         <v>562</v>
       </c>
       <c r="T21" t="s">
+        <v>660</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21" t="s">
         <v>663</v>
-      </c>
-      <c r="U21">
-        <v>1</v>
-      </c>
-      <c r="V21" t="s">
-        <v>666</v>
       </c>
       <c r="W21" t="s">
         <v>518</v>
@@ -3803,13 +3806,13 @@
         <v>562</v>
       </c>
       <c r="T22" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="U22">
         <v>3</v>
       </c>
       <c r="V22" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W22" t="s">
         <v>518</v>
@@ -3847,13 +3850,13 @@
         <v>562</v>
       </c>
       <c r="T23" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="U23">
         <v>1</v>
       </c>
       <c r="V23" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W23" t="s">
         <v>518</v>
@@ -3891,13 +3894,13 @@
         <v>562</v>
       </c>
       <c r="T24" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="U24">
         <v>3</v>
       </c>
       <c r="V24" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W24" t="s">
         <v>518</v>
@@ -3935,13 +3938,13 @@
         <v>562</v>
       </c>
       <c r="T25" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="U25">
         <v>3</v>
       </c>
       <c r="V25" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W25" t="s">
         <v>518</v>
@@ -3979,13 +3982,13 @@
         <v>562</v>
       </c>
       <c r="T26" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="U26">
         <v>3</v>
       </c>
       <c r="V26" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W26" t="s">
         <v>518</v>
@@ -4055,13 +4058,13 @@
         <v>562</v>
       </c>
       <c r="T28" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="U28">
         <v>11</v>
       </c>
       <c r="V28" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W28" t="s">
         <v>518</v>
@@ -4099,13 +4102,13 @@
         <v>562</v>
       </c>
       <c r="T29" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="U29">
         <v>12</v>
       </c>
       <c r="V29" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="W29" t="s">
         <v>518</v>
@@ -4143,13 +4146,13 @@
         <v>562</v>
       </c>
       <c r="T30" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="U30">
         <v>11</v>
       </c>
       <c r="V30" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W30" t="s">
         <v>518</v>
@@ -4187,13 +4190,13 @@
         <v>562</v>
       </c>
       <c r="T31" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="U31">
         <v>12</v>
       </c>
       <c r="V31" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="W31" t="s">
         <v>518</v>
@@ -4228,13 +4231,13 @@
         <v>562</v>
       </c>
       <c r="T32" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="U32">
         <v>11</v>
       </c>
       <c r="V32" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W32" t="s">
         <v>518</v>
@@ -4269,13 +4272,13 @@
         <v>562</v>
       </c>
       <c r="T33" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="U33">
         <v>12</v>
       </c>
       <c r="V33" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="W33" t="s">
         <v>518</v>
@@ -4313,13 +4316,13 @@
         <v>562</v>
       </c>
       <c r="T34" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="U34">
         <v>10</v>
       </c>
       <c r="V34" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W34" t="s">
         <v>518</v>
@@ -4439,13 +4442,13 @@
         <v>562</v>
       </c>
       <c r="T38" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="U38">
         <v>10</v>
       </c>
       <c r="V38" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W38" t="s">
         <v>518</v>
@@ -4518,13 +4521,13 @@
         <v>562</v>
       </c>
       <c r="T40" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="U40">
         <v>10</v>
       </c>
       <c r="V40" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W40" t="s">
         <v>518</v>
@@ -4594,13 +4597,13 @@
         <v>562</v>
       </c>
       <c r="T42" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="U42">
         <v>8</v>
       </c>
       <c r="V42" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W42" t="s">
         <v>518</v>
@@ -4667,13 +4670,13 @@
         <v>562</v>
       </c>
       <c r="T44" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="U44">
         <v>8</v>
       </c>
       <c r="V44" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W44" t="s">
         <v>518</v>
@@ -4743,13 +4746,13 @@
         <v>562</v>
       </c>
       <c r="T46" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="U46">
         <v>8</v>
       </c>
       <c r="V46" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W46" t="s">
         <v>518</v>
@@ -4819,13 +4822,13 @@
         <v>562</v>
       </c>
       <c r="T48" s="12" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="U48" s="12">
         <v>11</v>
       </c>
       <c r="V48" s="12" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W48" s="12" t="s">
         <v>518</v>
@@ -4896,13 +4899,13 @@
         <v>562</v>
       </c>
       <c r="T50" s="12" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="U50" s="12">
         <v>11</v>
       </c>
       <c r="V50" s="12" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W50" s="12" t="s">
         <v>518</v>
@@ -4970,13 +4973,13 @@
         <v>562</v>
       </c>
       <c r="T52" s="12" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="U52" s="12">
         <v>11</v>
       </c>
       <c r="V52" s="12" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W52" s="12" t="s">
         <v>518</v>
@@ -5151,13 +5154,13 @@
         <v>562</v>
       </c>
       <c r="T58" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="U58">
         <v>3</v>
       </c>
       <c r="V58" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W58" s="12" t="s">
         <v>518</v>
@@ -5198,13 +5201,13 @@
         <v>562</v>
       </c>
       <c r="T59" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="U59">
         <v>3</v>
       </c>
       <c r="V59" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W59" s="12" t="s">
         <v>518</v>
@@ -5245,13 +5248,13 @@
         <v>562</v>
       </c>
       <c r="T60" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="U60">
         <v>3</v>
       </c>
       <c r="V60" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W60" s="12" t="s">
         <v>518</v>
@@ -5286,13 +5289,13 @@
         <v>562</v>
       </c>
       <c r="T61" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="U61">
         <v>2</v>
       </c>
       <c r="V61" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W61" s="12" t="s">
         <v>518</v>
@@ -5333,13 +5336,13 @@
         <v>562</v>
       </c>
       <c r="T62" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="U62">
         <v>2</v>
       </c>
       <c r="V62" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
@@ -5374,13 +5377,13 @@
         <v>562</v>
       </c>
       <c r="T63" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="U63">
         <v>2</v>
       </c>
       <c r="V63" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
@@ -5415,13 +5418,13 @@
         <v>562</v>
       </c>
       <c r="T64" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="U64">
         <v>2</v>
       </c>
       <c r="V64" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.2">
@@ -5456,13 +5459,13 @@
         <v>562</v>
       </c>
       <c r="T65" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="U65">
         <v>2</v>
       </c>
       <c r="V65" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.2">
@@ -5497,13 +5500,13 @@
         <v>562</v>
       </c>
       <c r="T66" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="U66">
         <v>2</v>
       </c>
       <c r="V66" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.2">
@@ -5538,13 +5541,13 @@
         <v>562</v>
       </c>
       <c r="T67" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="U67">
         <v>2</v>
       </c>
       <c r="V67" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.2">
@@ -5579,13 +5582,13 @@
         <v>562</v>
       </c>
       <c r="T68" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="U68">
         <v>2</v>
       </c>
       <c r="V68" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.2">
@@ -5620,13 +5623,13 @@
         <v>562</v>
       </c>
       <c r="T69" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="U69">
         <v>2</v>
       </c>
       <c r="V69" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.2">
@@ -5661,13 +5664,13 @@
         <v>562</v>
       </c>
       <c r="T70" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="U70">
         <v>2</v>
       </c>
       <c r="V70" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.2">
@@ -5702,13 +5705,13 @@
         <v>562</v>
       </c>
       <c r="T71" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="U71">
         <v>2</v>
       </c>
       <c r="V71" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.2">
@@ -5743,13 +5746,13 @@
         <v>562</v>
       </c>
       <c r="T72" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="U72">
         <v>2</v>
       </c>
       <c r="V72" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.2">
@@ -5784,13 +5787,13 @@
         <v>562</v>
       </c>
       <c r="T73" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="U73">
         <v>2</v>
       </c>
       <c r="V73" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.2">
@@ -5825,13 +5828,13 @@
         <v>562</v>
       </c>
       <c r="T74" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="U74">
         <v>2</v>
       </c>
       <c r="V74" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.2">
@@ -6200,13 +6203,13 @@
         <v>244</v>
       </c>
       <c r="T89" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="U89">
         <v>3</v>
       </c>
       <c r="V89" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W89" t="s">
         <v>518</v>
@@ -6255,13 +6258,13 @@
         <v>248</v>
       </c>
       <c r="T91" t="s">
-        <v>674</v>
+        <v>712</v>
       </c>
       <c r="U91">
         <v>3</v>
       </c>
       <c r="V91" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W91" t="s">
         <v>518</v>
@@ -6310,13 +6313,13 @@
         <v>252</v>
       </c>
       <c r="T93" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="U93">
         <v>3</v>
       </c>
       <c r="V93" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W93" t="s">
         <v>518</v>
@@ -6635,7 +6638,7 @@
         <v>562</v>
       </c>
       <c r="T104" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="U104">
         <v>4</v>
@@ -6644,7 +6647,7 @@
         <v>486</v>
       </c>
       <c r="W104" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.2">
@@ -6708,7 +6711,7 @@
         <v>562</v>
       </c>
       <c r="T106" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="U106">
         <v>4</v>
@@ -6717,7 +6720,7 @@
         <v>486</v>
       </c>
       <c r="W106" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="107" spans="1:23" x14ac:dyDescent="0.2">
@@ -6790,7 +6793,7 @@
         <v>484</v>
       </c>
       <c r="W108" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="109" spans="1:23" x14ac:dyDescent="0.2">
@@ -6863,7 +6866,7 @@
         <v>484</v>
       </c>
       <c r="W110" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="111" spans="1:23" x14ac:dyDescent="0.2">
@@ -6936,7 +6939,7 @@
         <v>484</v>
       </c>
       <c r="W112" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="113" spans="1:23" x14ac:dyDescent="0.2">
@@ -6968,7 +6971,7 @@
         <v>46</v>
       </c>
       <c r="T113" t="s">
-        <v>626</v>
+        <v>708</v>
       </c>
       <c r="U113">
         <v>4</v>
@@ -6977,7 +6980,7 @@
         <v>486</v>
       </c>
       <c r="W113" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="114" spans="1:23" x14ac:dyDescent="0.2">
@@ -7021,7 +7024,7 @@
         <v>484</v>
       </c>
       <c r="W114" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="115" spans="1:23" x14ac:dyDescent="0.2">
@@ -7053,13 +7056,13 @@
         <v>46</v>
       </c>
       <c r="T115" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="U115">
         <v>3</v>
       </c>
       <c r="V115" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="W115" t="s">
         <v>518</v>
@@ -7150,7 +7153,7 @@
         <v>484</v>
       </c>
       <c r="W118" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="119" spans="1:23" x14ac:dyDescent="0.2">
@@ -7214,7 +7217,7 @@
         <v>562</v>
       </c>
       <c r="T120" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="U120">
         <v>4</v>
@@ -7223,7 +7226,7 @@
         <v>484</v>
       </c>
       <c r="W120" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="121" spans="1:23" x14ac:dyDescent="0.2">
@@ -7444,7 +7447,7 @@
         <v>46</v>
       </c>
       <c r="T127" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="U127">
         <v>5</v>
@@ -7453,7 +7456,7 @@
         <v>486</v>
       </c>
       <c r="W127" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="128" spans="1:23" x14ac:dyDescent="0.2">
@@ -7517,7 +7520,7 @@
         <v>46</v>
       </c>
       <c r="T129" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="U129">
         <v>5</v>
@@ -7526,7 +7529,7 @@
         <v>486</v>
       </c>
       <c r="W129" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="130" spans="1:23" x14ac:dyDescent="0.2">
@@ -7590,7 +7593,7 @@
         <v>46</v>
       </c>
       <c r="T131" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="U131">
         <v>5</v>
@@ -7599,7 +7602,7 @@
         <v>484</v>
       </c>
       <c r="W131" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="132" spans="1:23" x14ac:dyDescent="0.2">
@@ -7666,7 +7669,7 @@
         <v>46</v>
       </c>
       <c r="T133" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="U133">
         <v>5</v>
@@ -7675,7 +7678,7 @@
         <v>484</v>
       </c>
       <c r="W133" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="134" spans="1:23" x14ac:dyDescent="0.2">
@@ -7709,6 +7712,9 @@
       <c r="R134" t="s">
         <v>562</v>
       </c>
+      <c r="T134" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="135" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
@@ -7742,7 +7748,7 @@
         <v>46</v>
       </c>
       <c r="T135" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="U135">
         <v>5</v>
@@ -7751,7 +7757,7 @@
         <v>484</v>
       </c>
       <c r="W135" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="136" spans="1:23" x14ac:dyDescent="0.2">
@@ -7830,7 +7836,7 @@
         <v>562</v>
       </c>
       <c r="T138" t="s">
-        <v>637</v>
+        <v>709</v>
       </c>
       <c r="U138">
         <v>5</v>
@@ -7839,7 +7845,7 @@
         <v>486</v>
       </c>
       <c r="W138" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="139" spans="1:23" x14ac:dyDescent="0.2">
@@ -7874,7 +7880,7 @@
         <v>46</v>
       </c>
       <c r="T139" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="U139">
         <v>5</v>
@@ -7883,7 +7889,7 @@
         <v>484</v>
       </c>
       <c r="W139" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="140" spans="1:23" x14ac:dyDescent="0.2">
@@ -7921,7 +7927,7 @@
         <v>562</v>
       </c>
       <c r="T140" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="U140">
         <v>5</v>
@@ -7930,7 +7936,7 @@
         <v>484</v>
       </c>
       <c r="W140" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="141" spans="1:23" x14ac:dyDescent="0.2">
@@ -7965,7 +7971,7 @@
         <v>46</v>
       </c>
       <c r="T141" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="U141">
         <v>7</v>
@@ -7974,7 +7980,7 @@
         <v>486</v>
       </c>
       <c r="W141" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="142" spans="1:23" x14ac:dyDescent="0.2">
@@ -8012,7 +8018,7 @@
         <v>562</v>
       </c>
       <c r="T142" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="U142">
         <v>5</v>
@@ -8021,7 +8027,7 @@
         <v>484</v>
       </c>
       <c r="W142" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="143" spans="1:23" x14ac:dyDescent="0.2">
@@ -8056,7 +8062,7 @@
         <v>46</v>
       </c>
       <c r="T143" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="U143">
         <v>7</v>
@@ -8065,7 +8071,7 @@
         <v>486</v>
       </c>
       <c r="W143" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="144" spans="1:23" x14ac:dyDescent="0.2">
@@ -8103,7 +8109,7 @@
         <v>562</v>
       </c>
       <c r="T144" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="U144">
         <v>6</v>
@@ -8112,7 +8118,7 @@
         <v>486</v>
       </c>
       <c r="W144" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="145" spans="1:23" x14ac:dyDescent="0.2">
@@ -8150,7 +8156,7 @@
         <v>46</v>
       </c>
       <c r="T145" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="U145">
         <v>7</v>
@@ -8159,7 +8165,7 @@
         <v>484</v>
       </c>
       <c r="W145" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="146" spans="1:23" x14ac:dyDescent="0.2">
@@ -8197,7 +8203,7 @@
         <v>562</v>
       </c>
       <c r="T146" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="U146">
         <v>6</v>
@@ -8206,7 +8212,7 @@
         <v>486</v>
       </c>
       <c r="W146" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="147" spans="1:23" x14ac:dyDescent="0.2">
@@ -8244,7 +8250,7 @@
         <v>46</v>
       </c>
       <c r="T147" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="U147">
         <v>7</v>
@@ -8253,7 +8259,7 @@
         <v>484</v>
       </c>
       <c r="W147" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="148" spans="1:23" x14ac:dyDescent="0.2">
@@ -8291,7 +8297,7 @@
         <v>562</v>
       </c>
       <c r="T148" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="U148">
         <v>6</v>
@@ -8300,7 +8306,7 @@
         <v>484</v>
       </c>
       <c r="W148" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="149" spans="1:23" x14ac:dyDescent="0.2">
@@ -8338,7 +8344,7 @@
         <v>562</v>
       </c>
       <c r="T149" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="U149">
         <v>7</v>
@@ -8347,7 +8353,7 @@
         <v>484</v>
       </c>
       <c r="W149" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="150" spans="1:23" x14ac:dyDescent="0.2">
@@ -8385,7 +8391,7 @@
         <v>562</v>
       </c>
       <c r="T150" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="U150">
         <v>6</v>
@@ -8394,7 +8400,7 @@
         <v>484</v>
       </c>
       <c r="W150" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="151" spans="1:23" x14ac:dyDescent="0.2">
@@ -8432,7 +8438,7 @@
         <v>562</v>
       </c>
       <c r="T151" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="U151" s="12">
         <v>7</v>
@@ -8441,7 +8447,7 @@
         <v>484</v>
       </c>
       <c r="W151" s="12" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="152" spans="1:23" x14ac:dyDescent="0.2">
@@ -8479,7 +8485,7 @@
         <v>562</v>
       </c>
       <c r="T152" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="U152">
         <v>6</v>
@@ -8488,7 +8494,7 @@
         <v>484</v>
       </c>
       <c r="W152" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="153" spans="1:23" x14ac:dyDescent="0.2">
@@ -8526,7 +8532,7 @@
         <v>562</v>
       </c>
       <c r="T153" t="s">
-        <v>646</v>
+        <v>710</v>
       </c>
       <c r="U153">
         <v>6</v>
@@ -8535,7 +8541,7 @@
         <v>486</v>
       </c>
       <c r="W153" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="154" spans="1:23" x14ac:dyDescent="0.2">
@@ -8573,7 +8579,7 @@
         <v>562</v>
       </c>
       <c r="T154" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="U154">
         <v>6</v>
@@ -8582,7 +8588,7 @@
         <v>484</v>
       </c>
       <c r="W154" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="155" spans="1:23" x14ac:dyDescent="0.2">
@@ -8620,7 +8626,7 @@
         <v>562</v>
       </c>
       <c r="T155" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="U155">
         <v>7</v>
@@ -8629,7 +8635,7 @@
         <v>486</v>
       </c>
       <c r="W155" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="156" spans="1:23" x14ac:dyDescent="0.2">
@@ -8667,7 +8673,7 @@
         <v>562</v>
       </c>
       <c r="T156" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="U156">
         <v>6</v>
@@ -8676,7 +8682,7 @@
         <v>484</v>
       </c>
       <c r="W156" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="157" spans="1:23" x14ac:dyDescent="0.2">
@@ -8714,7 +8720,7 @@
         <v>562</v>
       </c>
       <c r="T157" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="U157">
         <v>6</v>
@@ -8723,7 +8729,7 @@
         <v>484</v>
       </c>
       <c r="W157" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="158" spans="1:23" x14ac:dyDescent="0.2">
@@ -8764,7 +8770,7 @@
         <v>562</v>
       </c>
       <c r="T158" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="U158">
         <v>7</v>
@@ -8773,7 +8779,7 @@
         <v>484</v>
       </c>
       <c r="W158" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="159" spans="1:23" x14ac:dyDescent="0.2">
@@ -8834,7 +8840,7 @@
         <v>562</v>
       </c>
       <c r="T160" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="U160">
         <v>7</v>
@@ -8843,7 +8849,7 @@
         <v>484</v>
       </c>
       <c r="W160" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
v1 final edits; creating tag
</commit_message>
<xml_diff>
--- a/documentation/signals/XEM6310.xlsx
+++ b/documentation/signals/XEM6310.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/eagle/projects/open_covg_daq_pcb/documentation/signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5E150E-C6D2-4B40-ACDB-E1AC63E50BFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9CA1A8-DE43-1749-8B48-97CCA3377B24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="29780" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XEM6310" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="714">
   <si>
     <t>Connector</t>
   </si>
@@ -1947,12 +1947,6 @@
     <t>ADP2300</t>
   </si>
   <si>
-    <t>lvds</t>
-  </si>
-  <si>
-    <t>lvcmos</t>
-  </si>
-  <si>
     <t>Schematic sheet</t>
   </si>
   <si>
@@ -2221,6 +2215,15 @@
   </si>
   <si>
     <t>A3_CLK_N</t>
+  </si>
+  <si>
+    <t>IOStandard</t>
+  </si>
+  <si>
+    <t>LVCMOS33</t>
+  </si>
+  <si>
+    <t>DiffTerm</t>
   </si>
 </sst>
 </file>
@@ -3129,10 +3132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W161"/>
+  <dimension ref="A1:X161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T161" sqref="T161"/>
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3150,7 +3153,7 @@
     <col min="22" max="22" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3206,16 +3209,22 @@
         <v>561</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+        <v>622</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -3235,7 +3244,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3255,7 +3264,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3275,7 +3284,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -3295,7 +3304,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3315,7 +3324,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3335,7 +3344,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -3355,7 +3364,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3375,7 +3384,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3395,7 +3404,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3418,7 +3427,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3447,19 +3456,19 @@
         <v>564</v>
       </c>
       <c r="T12" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="U12">
         <v>3</v>
       </c>
       <c r="V12" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W12" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3482,7 +3491,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3505,7 +3514,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -3528,7 +3537,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -3592,16 +3601,16 @@
         <v>562</v>
       </c>
       <c r="T17" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="U17">
         <v>1</v>
       </c>
       <c r="V17" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="W17" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
@@ -3636,16 +3645,16 @@
         <v>562</v>
       </c>
       <c r="T18" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="U18">
         <v>3</v>
       </c>
       <c r="V18" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W18" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
@@ -3680,16 +3689,16 @@
         <v>562</v>
       </c>
       <c r="T19" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="U19">
         <v>1</v>
       </c>
       <c r="V19" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W19" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
@@ -3721,16 +3730,16 @@
         <v>562</v>
       </c>
       <c r="T20" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="U20">
         <v>3</v>
       </c>
       <c r="V20" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W20" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
@@ -3762,16 +3771,16 @@
         <v>562</v>
       </c>
       <c r="T21" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="U21">
         <v>1</v>
       </c>
       <c r="V21" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W21" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
@@ -3806,16 +3815,16 @@
         <v>562</v>
       </c>
       <c r="T22" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="U22">
         <v>3</v>
       </c>
       <c r="V22" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W22" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
@@ -3850,16 +3859,16 @@
         <v>562</v>
       </c>
       <c r="T23" t="s">
+        <v>627</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23" t="s">
         <v>629</v>
       </c>
-      <c r="U23">
-        <v>1</v>
-      </c>
-      <c r="V23" t="s">
-        <v>631</v>
-      </c>
       <c r="W23" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
@@ -3894,16 +3903,16 @@
         <v>562</v>
       </c>
       <c r="T24" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="U24">
         <v>3</v>
       </c>
       <c r="V24" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W24" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
@@ -3938,16 +3947,16 @@
         <v>562</v>
       </c>
       <c r="T25" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="U25">
         <v>3</v>
       </c>
       <c r="V25" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W25" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -3982,16 +3991,16 @@
         <v>562</v>
       </c>
       <c r="T26" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="U26">
         <v>3</v>
       </c>
       <c r="V26" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W26" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
@@ -4058,16 +4067,16 @@
         <v>562</v>
       </c>
       <c r="T28" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="U28">
         <v>11</v>
       </c>
       <c r="V28" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W28" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
@@ -4102,16 +4111,16 @@
         <v>562</v>
       </c>
       <c r="T29" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="U29">
         <v>12</v>
       </c>
       <c r="V29" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="W29" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
@@ -4146,16 +4155,16 @@
         <v>562</v>
       </c>
       <c r="T30" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="U30">
         <v>11</v>
       </c>
       <c r="V30" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W30" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
@@ -4190,16 +4199,16 @@
         <v>562</v>
       </c>
       <c r="T31" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="U31">
         <v>12</v>
       </c>
       <c r="V31" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="W31" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
@@ -4231,16 +4240,16 @@
         <v>562</v>
       </c>
       <c r="T32" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="U32">
         <v>11</v>
       </c>
       <c r="V32" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W32" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
@@ -4272,16 +4281,16 @@
         <v>562</v>
       </c>
       <c r="T33" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="U33">
         <v>12</v>
       </c>
       <c r="V33" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="W33" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
@@ -4316,16 +4325,16 @@
         <v>562</v>
       </c>
       <c r="T34" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="U34">
         <v>10</v>
       </c>
       <c r="V34" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W34" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
@@ -4442,16 +4451,16 @@
         <v>562</v>
       </c>
       <c r="T38" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="U38">
         <v>10</v>
       </c>
       <c r="V38" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W38" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
@@ -4521,16 +4530,16 @@
         <v>562</v>
       </c>
       <c r="T40" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="U40">
         <v>10</v>
       </c>
       <c r="V40" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W40" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
@@ -4597,16 +4606,16 @@
         <v>562</v>
       </c>
       <c r="T42" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="U42">
         <v>8</v>
       </c>
       <c r="V42" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W42" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
@@ -4670,16 +4679,16 @@
         <v>562</v>
       </c>
       <c r="T44" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="U44">
         <v>8</v>
       </c>
       <c r="V44" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W44" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
@@ -4746,16 +4755,16 @@
         <v>562</v>
       </c>
       <c r="T46" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="U46">
         <v>8</v>
       </c>
       <c r="V46" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W46" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
@@ -4822,16 +4831,16 @@
         <v>562</v>
       </c>
       <c r="T48" s="12" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="U48" s="12">
         <v>11</v>
       </c>
       <c r="V48" s="12" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W48" s="12" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
@@ -4899,16 +4908,16 @@
         <v>562</v>
       </c>
       <c r="T50" s="12" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="U50" s="12">
         <v>11</v>
       </c>
       <c r="V50" s="12" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W50" s="12" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
@@ -4973,16 +4982,16 @@
         <v>562</v>
       </c>
       <c r="T52" s="12" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="U52" s="12">
         <v>11</v>
       </c>
       <c r="V52" s="12" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W52" s="12" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
@@ -5154,16 +5163,16 @@
         <v>562</v>
       </c>
       <c r="T58" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="U58">
         <v>3</v>
       </c>
       <c r="V58" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W58" s="12" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
@@ -5201,16 +5210,16 @@
         <v>562</v>
       </c>
       <c r="T59" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="U59">
         <v>3</v>
       </c>
       <c r="V59" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W59" s="12" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
@@ -5248,16 +5257,16 @@
         <v>562</v>
       </c>
       <c r="T60" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="U60">
         <v>3</v>
       </c>
       <c r="V60" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W60" s="12" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
@@ -5289,16 +5298,16 @@
         <v>562</v>
       </c>
       <c r="T61" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="U61">
         <v>2</v>
       </c>
       <c r="V61" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W61" s="12" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.2">
@@ -5336,13 +5345,13 @@
         <v>562</v>
       </c>
       <c r="T62" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="U62">
         <v>2</v>
       </c>
       <c r="V62" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
@@ -5377,13 +5386,13 @@
         <v>562</v>
       </c>
       <c r="T63" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U63">
         <v>2</v>
       </c>
       <c r="V63" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
@@ -5418,13 +5427,13 @@
         <v>562</v>
       </c>
       <c r="T64" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="U64">
         <v>2</v>
       </c>
       <c r="V64" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.2">
@@ -5459,13 +5468,13 @@
         <v>562</v>
       </c>
       <c r="T65" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="U65">
         <v>2</v>
       </c>
       <c r="V65" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.2">
@@ -5500,13 +5509,13 @@
         <v>562</v>
       </c>
       <c r="T66" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="U66">
         <v>2</v>
       </c>
       <c r="V66" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.2">
@@ -5541,13 +5550,13 @@
         <v>562</v>
       </c>
       <c r="T67" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="U67">
         <v>2</v>
       </c>
       <c r="V67" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.2">
@@ -5582,13 +5591,13 @@
         <v>562</v>
       </c>
       <c r="T68" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="U68">
         <v>2</v>
       </c>
       <c r="V68" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.2">
@@ -5623,13 +5632,13 @@
         <v>562</v>
       </c>
       <c r="T69" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="U69">
         <v>2</v>
       </c>
       <c r="V69" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.2">
@@ -5664,13 +5673,13 @@
         <v>562</v>
       </c>
       <c r="T70" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="U70">
         <v>2</v>
       </c>
       <c r="V70" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.2">
@@ -5705,13 +5714,13 @@
         <v>562</v>
       </c>
       <c r="T71" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="U71">
         <v>2</v>
       </c>
       <c r="V71" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.2">
@@ -5746,13 +5755,13 @@
         <v>562</v>
       </c>
       <c r="T72" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="U72">
         <v>2</v>
       </c>
       <c r="V72" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.2">
@@ -5787,13 +5796,13 @@
         <v>562</v>
       </c>
       <c r="T73" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="U73">
         <v>2</v>
       </c>
       <c r="V73" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.2">
@@ -5828,13 +5837,13 @@
         <v>562</v>
       </c>
       <c r="T74" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="U74">
         <v>2</v>
       </c>
       <c r="V74" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.2">
@@ -6203,16 +6212,16 @@
         <v>244</v>
       </c>
       <c r="T89" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="U89">
         <v>3</v>
       </c>
       <c r="V89" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W89" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.2">
@@ -6258,16 +6267,16 @@
         <v>248</v>
       </c>
       <c r="T91" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="U91">
         <v>3</v>
       </c>
       <c r="V91" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W91" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.2">
@@ -6313,16 +6322,16 @@
         <v>252</v>
       </c>
       <c r="T93" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="U93">
         <v>3</v>
       </c>
       <c r="V93" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W93" t="s">
-        <v>518</v>
+        <v>712</v>
       </c>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.2">
@@ -6394,7 +6403,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>232</v>
       </c>
@@ -6423,7 +6432,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>232</v>
       </c>
@@ -6455,7 +6464,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>232</v>
       </c>
@@ -6484,7 +6493,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>232</v>
       </c>
@@ -6516,7 +6525,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>232</v>
       </c>
@@ -6545,7 +6554,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>232</v>
       </c>
@@ -6577,7 +6586,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>232</v>
       </c>
@@ -6606,7 +6615,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>232</v>
       </c>
@@ -6638,7 +6647,7 @@
         <v>562</v>
       </c>
       <c r="T104" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="U104">
         <v>4</v>
@@ -6647,10 +6656,10 @@
         <v>486</v>
       </c>
       <c r="W104" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>232</v>
       </c>
@@ -6679,7 +6688,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>232</v>
       </c>
@@ -6711,7 +6720,7 @@
         <v>562</v>
       </c>
       <c r="T106" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="U106">
         <v>4</v>
@@ -6720,10 +6729,10 @@
         <v>486</v>
       </c>
       <c r="W106" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>232</v>
       </c>
@@ -6752,7 +6761,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>232</v>
       </c>
@@ -6784,7 +6793,7 @@
         <v>562</v>
       </c>
       <c r="T108" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="U108">
         <v>4</v>
@@ -6793,10 +6802,13 @@
         <v>484</v>
       </c>
       <c r="W108" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>232</v>
       </c>
@@ -6825,7 +6837,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>232</v>
       </c>
@@ -6857,7 +6869,7 @@
         <v>562</v>
       </c>
       <c r="T110" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="U110">
         <v>4</v>
@@ -6866,10 +6878,13 @@
         <v>484</v>
       </c>
       <c r="W110" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>232</v>
       </c>
@@ -6898,7 +6913,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>232</v>
       </c>
@@ -6930,7 +6945,7 @@
         <v>562</v>
       </c>
       <c r="T112" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="U112">
         <v>4</v>
@@ -6939,10 +6954,13 @@
         <v>484</v>
       </c>
       <c r="W112" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>232</v>
       </c>
@@ -6971,7 +6989,7 @@
         <v>46</v>
       </c>
       <c r="T113" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="U113">
         <v>4</v>
@@ -6980,10 +6998,10 @@
         <v>486</v>
       </c>
       <c r="W113" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.2">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>232</v>
       </c>
@@ -7015,7 +7033,7 @@
         <v>562</v>
       </c>
       <c r="T114" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="U114">
         <v>4</v>
@@ -7024,10 +7042,13 @@
         <v>484</v>
       </c>
       <c r="W114" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>232</v>
       </c>
@@ -7056,19 +7077,19 @@
         <v>46</v>
       </c>
       <c r="T115" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="U115">
         <v>3</v>
       </c>
       <c r="V115" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="W115" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.2">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>232</v>
       </c>
@@ -7088,7 +7109,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>232</v>
       </c>
@@ -7112,7 +7133,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>232</v>
       </c>
@@ -7144,7 +7165,7 @@
         <v>562</v>
       </c>
       <c r="T118" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="U118">
         <v>4</v>
@@ -7153,10 +7174,10 @@
         <v>484</v>
       </c>
       <c r="W118" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>232</v>
       </c>
@@ -7185,7 +7206,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>232</v>
       </c>
@@ -7217,7 +7238,7 @@
         <v>562</v>
       </c>
       <c r="T120" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="U120">
         <v>4</v>
@@ -7226,10 +7247,10 @@
         <v>484</v>
       </c>
       <c r="W120" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>232</v>
       </c>
@@ -7258,7 +7279,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>232</v>
       </c>
@@ -7290,7 +7311,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>232</v>
       </c>
@@ -7322,7 +7343,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>232</v>
       </c>
@@ -7354,7 +7375,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>232</v>
       </c>
@@ -7386,7 +7407,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>232</v>
       </c>
@@ -7418,7 +7439,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>232</v>
       </c>
@@ -7447,7 +7468,7 @@
         <v>46</v>
       </c>
       <c r="T127" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="U127">
         <v>5</v>
@@ -7456,10 +7477,10 @@
         <v>486</v>
       </c>
       <c r="W127" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="128" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>232</v>
       </c>
@@ -7491,7 +7512,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>232</v>
       </c>
@@ -7520,7 +7541,7 @@
         <v>46</v>
       </c>
       <c r="T129" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="U129">
         <v>5</v>
@@ -7529,10 +7550,10 @@
         <v>486</v>
       </c>
       <c r="W129" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>232</v>
       </c>
@@ -7564,7 +7585,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>232</v>
       </c>
@@ -7593,7 +7614,7 @@
         <v>46</v>
       </c>
       <c r="T131" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="U131">
         <v>5</v>
@@ -7602,10 +7623,13 @@
         <v>484</v>
       </c>
       <c r="W131" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>232</v>
       </c>
@@ -7637,7 +7661,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>232</v>
       </c>
@@ -7669,7 +7693,7 @@
         <v>46</v>
       </c>
       <c r="T133" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="U133">
         <v>5</v>
@@ -7678,10 +7702,13 @@
         <v>484</v>
       </c>
       <c r="W133" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>232</v>
       </c>
@@ -7713,10 +7740,10 @@
         <v>562</v>
       </c>
       <c r="T134" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.2">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="135" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>232</v>
       </c>
@@ -7748,7 +7775,7 @@
         <v>46</v>
       </c>
       <c r="T135" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="U135">
         <v>5</v>
@@ -7757,10 +7784,13 @@
         <v>484</v>
       </c>
       <c r="W135" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>232</v>
       </c>
@@ -7780,7 +7810,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>232</v>
       </c>
@@ -7804,7 +7834,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>232</v>
       </c>
@@ -7836,7 +7866,7 @@
         <v>562</v>
       </c>
       <c r="T138" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="U138">
         <v>5</v>
@@ -7845,10 +7875,10 @@
         <v>486</v>
       </c>
       <c r="W138" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.2">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="139" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>232</v>
       </c>
@@ -7880,7 +7910,7 @@
         <v>46</v>
       </c>
       <c r="T139" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="U139">
         <v>5</v>
@@ -7889,10 +7919,13 @@
         <v>484</v>
       </c>
       <c r="W139" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X139" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>232</v>
       </c>
@@ -7927,7 +7960,7 @@
         <v>562</v>
       </c>
       <c r="T140" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="U140">
         <v>5</v>
@@ -7936,10 +7969,10 @@
         <v>484</v>
       </c>
       <c r="W140" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="141" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>232</v>
       </c>
@@ -7971,7 +8004,7 @@
         <v>46</v>
       </c>
       <c r="T141" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="U141">
         <v>7</v>
@@ -7980,10 +8013,10 @@
         <v>486</v>
       </c>
       <c r="W141" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="142" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>232</v>
       </c>
@@ -8018,7 +8051,7 @@
         <v>562</v>
       </c>
       <c r="T142" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="U142">
         <v>5</v>
@@ -8027,10 +8060,10 @@
         <v>484</v>
       </c>
       <c r="W142" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="143" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>232</v>
       </c>
@@ -8062,7 +8095,7 @@
         <v>46</v>
       </c>
       <c r="T143" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="U143">
         <v>7</v>
@@ -8071,10 +8104,10 @@
         <v>486</v>
       </c>
       <c r="W143" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="144" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>232</v>
       </c>
@@ -8109,7 +8142,7 @@
         <v>562</v>
       </c>
       <c r="T144" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="U144">
         <v>6</v>
@@ -8118,10 +8151,10 @@
         <v>486</v>
       </c>
       <c r="W144" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="145" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>232</v>
       </c>
@@ -8156,7 +8189,7 @@
         <v>46</v>
       </c>
       <c r="T145" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="U145">
         <v>7</v>
@@ -8165,10 +8198,13 @@
         <v>484</v>
       </c>
       <c r="W145" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>232</v>
       </c>
@@ -8203,7 +8239,7 @@
         <v>562</v>
       </c>
       <c r="T146" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="U146">
         <v>6</v>
@@ -8212,10 +8248,10 @@
         <v>486</v>
       </c>
       <c r="W146" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="147" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>232</v>
       </c>
@@ -8250,7 +8286,7 @@
         <v>46</v>
       </c>
       <c r="T147" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="U147">
         <v>7</v>
@@ -8259,10 +8295,13 @@
         <v>484</v>
       </c>
       <c r="W147" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X147" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>232</v>
       </c>
@@ -8297,7 +8336,7 @@
         <v>562</v>
       </c>
       <c r="T148" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="U148">
         <v>6</v>
@@ -8306,10 +8345,13 @@
         <v>484</v>
       </c>
       <c r="W148" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>232</v>
       </c>
@@ -8344,7 +8386,7 @@
         <v>562</v>
       </c>
       <c r="T149" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="U149">
         <v>7</v>
@@ -8353,10 +8395,13 @@
         <v>484</v>
       </c>
       <c r="W149" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>232</v>
       </c>
@@ -8391,7 +8436,7 @@
         <v>562</v>
       </c>
       <c r="T150" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="U150">
         <v>6</v>
@@ -8400,10 +8445,13 @@
         <v>484</v>
       </c>
       <c r="W150" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>232</v>
       </c>
@@ -8438,7 +8486,7 @@
         <v>562</v>
       </c>
       <c r="T151" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="U151" s="12">
         <v>7</v>
@@ -8447,10 +8495,13 @@
         <v>484</v>
       </c>
       <c r="W151" s="12" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X151" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>232</v>
       </c>
@@ -8485,7 +8536,7 @@
         <v>562</v>
       </c>
       <c r="T152" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="U152">
         <v>6</v>
@@ -8494,10 +8545,13 @@
         <v>484</v>
       </c>
       <c r="W152" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>232</v>
       </c>
@@ -8532,7 +8586,7 @@
         <v>562</v>
       </c>
       <c r="T153" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="U153">
         <v>6</v>
@@ -8541,10 +8595,10 @@
         <v>486</v>
       </c>
       <c r="W153" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.2">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="154" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>232</v>
       </c>
@@ -8579,7 +8633,7 @@
         <v>562</v>
       </c>
       <c r="T154" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="U154">
         <v>6</v>
@@ -8588,10 +8642,13 @@
         <v>484</v>
       </c>
       <c r="W154" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+      <c r="X154" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>232</v>
       </c>
@@ -8626,7 +8683,7 @@
         <v>562</v>
       </c>
       <c r="T155" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="U155">
         <v>7</v>
@@ -8635,10 +8692,10 @@
         <v>486</v>
       </c>
       <c r="W155" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.2">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="156" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>232</v>
       </c>
@@ -8673,7 +8730,7 @@
         <v>562</v>
       </c>
       <c r="T156" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="U156">
         <v>6</v>
@@ -8682,10 +8739,10 @@
         <v>484</v>
       </c>
       <c r="W156" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="157" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>232</v>
       </c>
@@ -8720,7 +8777,7 @@
         <v>562</v>
       </c>
       <c r="T157" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="U157">
         <v>6</v>
@@ -8729,10 +8786,10 @@
         <v>484</v>
       </c>
       <c r="W157" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="158" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>232</v>
       </c>
@@ -8770,7 +8827,7 @@
         <v>562</v>
       </c>
       <c r="T158" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="U158">
         <v>7</v>
@@ -8779,10 +8836,10 @@
         <v>484</v>
       </c>
       <c r="W158" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="159" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>232</v>
       </c>
@@ -8802,7 +8859,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>232</v>
       </c>
@@ -8840,7 +8897,7 @@
         <v>562</v>
       </c>
       <c r="T160" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U160">
         <v>7</v>
@@ -8849,7 +8906,7 @@
         <v>484</v>
       </c>
       <c r="W160" t="s">
-        <v>621</v>
+        <v>495</v>
       </c>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>